<commit_message>
Update 000018 PGKB Rev 3.00 BOM_purchasing.xlsx
</commit_message>
<xml_diff>
--- a/PCB/Rev 03.00/000018 PGKB/MFG/000018 PGKB Rev 3.00 BOM_purchasing.xlsx
+++ b/PCB/Rev 03.00/000018 PGKB/MFG/000018 PGKB Rev 3.00 BOM_purchasing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubProjects\PGKB\PCB\Rev 03.00\000018 PGKB\MFG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD7304D-F87E-4E10-A3AE-59B928C40CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6A0F9B-B11E-4F1A-9561-694209A9A241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="16650" windowHeight="14625" xr2:uid="{86873884-B4BD-499F-83C6-413FB57D0B81}"/>
+    <workbookView xWindow="10005" yWindow="600" windowWidth="16650" windowHeight="14625" xr2:uid="{86873884-B4BD-499F-83C6-413FB57D0B81}"/>
   </bookViews>
   <sheets>
     <sheet name="000018 PGKB Rev 3.00 BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="163">
   <si>
     <t>Reference</t>
   </si>
@@ -500,48 +500,6 @@
   </si>
   <si>
     <t>BAT54WSQ-7-FDICT-ND</t>
-  </si>
-  <si>
-    <t>H1,H2,H4</t>
-  </si>
-  <si>
-    <t>NPTH 3.2 M3 Clearance</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>H3</t>
-  </si>
-  <si>
-    <t>NPTH_3.2</t>
-  </si>
-  <si>
-    <t>H5,H6</t>
-  </si>
-  <si>
-    <t>PTH 3.2 M3 Clearance</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>GND Hook</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>TP1,TP2,TP3,TP4,TP5,TP6,TP7,TP8,TP10,TP11,TP12,TP13,TP14,TP15,TP16,TP17</t>
-  </si>
-  <si>
-    <t>TP D2.5 mm H0.9mm</t>
-  </si>
-  <si>
-    <t>TP9</t>
-  </si>
-  <si>
-    <t>TestPoint_1.5mm_Round</t>
   </si>
   <si>
     <t>APX811-31UG-7</t>
@@ -1411,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A42D5893-558B-4E0C-9CD4-B2E5B941F3D3}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,28 +1801,31 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>162</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I14" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="J14" t="s">
         <v>153</v>
@@ -1872,28 +1833,31 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>162</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="G15" t="s">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="H15" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I15" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="J15" t="s">
         <v>153</v>
@@ -1901,28 +1865,31 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>147</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>162</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="G16" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="H16" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="J16" t="s">
         <v>153</v>
@@ -1930,31 +1897,31 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" t="s">
-        <v>73</v>
+        <v>88</v>
+      </c>
+      <c r="B17">
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G17" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="J17" t="s">
         <v>153</v>
@@ -1962,31 +1929,31 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H18" t="s">
         <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="J18" t="s">
         <v>153</v>
@@ -1994,28 +1961,31 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>167</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>168</v>
+        <v>99</v>
+      </c>
+      <c r="C19" t="s">
+        <v>95</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>162</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="H19" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I19" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="J19" t="s">
         <v>153</v>
@@ -2023,22 +1993,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="C20" t="s">
         <v>84</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="G20" t="s">
         <v>86</v>
@@ -2047,7 +2017,7 @@
         <v>15</v>
       </c>
       <c r="I20" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="J20" t="s">
         <v>153</v>
@@ -2055,13 +2025,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="B21">
-        <v>27</v>
+        <v>360</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -2070,16 +2040,16 @@
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="G21" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="H21" t="s">
         <v>15</v>
       </c>
       <c r="I21" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="J21" t="s">
         <v>153</v>
@@ -2087,121 +2057,133 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" t="s">
-        <v>94</v>
+        <v>111</v>
+      </c>
+      <c r="B22">
+        <v>4958</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="D22">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
       </c>
-      <c r="F22" t="s">
-        <v>96</v>
+      <c r="F22">
+        <v>4958</v>
       </c>
       <c r="G22" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="H22" t="s">
         <v>15</v>
       </c>
       <c r="I22" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="J22" t="s">
         <v>153</v>
+      </c>
+      <c r="K22" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
       <c r="C23" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="D23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="G23" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
       <c r="H23" t="s">
         <v>15</v>
       </c>
       <c r="I23" t="s">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="J23" t="s">
         <v>153</v>
+      </c>
+      <c r="K23" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>169</v>
-      </c>
-      <c r="B24" t="s">
-        <v>4</v>
+        <v>154</v>
+      </c>
+      <c r="B24">
+        <v>4954</v>
+      </c>
+      <c r="C24" t="s">
+        <v>155</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>162</v>
-      </c>
-      <c r="F24" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>4954</v>
       </c>
       <c r="G24" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="H24" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I24" t="s">
-        <v>4</v>
+        <v>156</v>
+      </c>
+      <c r="J24" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="D25">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="G25" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H25" t="s">
         <v>15</v>
       </c>
       <c r="I25" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="J25" t="s">
         <v>153</v>
@@ -2209,31 +2191,31 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>106</v>
-      </c>
-      <c r="B26">
-        <v>360</v>
+        <v>120</v>
+      </c>
+      <c r="B26" t="s">
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G26" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="H26" t="s">
         <v>15</v>
       </c>
       <c r="I26" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="J26" t="s">
         <v>153</v>
@@ -2241,13 +2223,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>111</v>
-      </c>
-      <c r="B27">
-        <v>4958</v>
+        <v>125</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2255,87 +2237,81 @@
       <c r="E27" t="s">
         <v>12</v>
       </c>
-      <c r="F27">
-        <v>4958</v>
+      <c r="F27" t="s">
+        <v>126</v>
       </c>
       <c r="G27" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="H27" t="s">
         <v>15</v>
       </c>
       <c r="I27" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="J27" t="s">
         <v>153</v>
-      </c>
-      <c r="K27" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="G28" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="H28" t="s">
         <v>15</v>
       </c>
       <c r="I28" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="J28" t="s">
         <v>153</v>
-      </c>
-      <c r="K28" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>154</v>
-      </c>
-      <c r="B29">
-        <v>4954</v>
+        <v>136</v>
+      </c>
+      <c r="B29" t="s">
+        <v>137</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
       </c>
-      <c r="F29">
-        <v>4954</v>
+      <c r="F29" t="s">
+        <v>137</v>
       </c>
       <c r="G29" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="H29" t="s">
         <v>15</v>
       </c>
       <c r="I29" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="J29" t="s">
         <v>153</v>
@@ -2343,13 +2319,13 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -2358,16 +2334,16 @@
         <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="G30" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="H30" t="s">
         <v>15</v>
       </c>
       <c r="I30" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="J30" t="s">
         <v>153</v>
@@ -2375,237 +2351,34 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
       <c r="D31">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>162</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>4</v>
+        <v>145</v>
       </c>
       <c r="G31" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="H31" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I31" t="s">
-        <v>4</v>
+        <v>146</v>
       </c>
       <c r="J31" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>172</v>
-      </c>
-      <c r="B32" t="s">
-        <v>173</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>162</v>
-      </c>
-      <c r="F32" t="s">
-        <v>4</v>
-      </c>
-      <c r="G32" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" t="s">
-        <v>121</v>
-      </c>
-      <c r="C33" t="s">
-        <v>122</v>
-      </c>
-      <c r="D33">
-        <v>3</v>
-      </c>
-      <c r="E33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" t="s">
-        <v>121</v>
-      </c>
-      <c r="G33" t="s">
-        <v>123</v>
-      </c>
-      <c r="H33" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>125</v>
-      </c>
-      <c r="B34" t="s">
-        <v>126</v>
-      </c>
-      <c r="C34" t="s">
-        <v>127</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" t="s">
-        <v>126</v>
-      </c>
-      <c r="G34" t="s">
-        <v>128</v>
-      </c>
-      <c r="H34" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>130</v>
-      </c>
-      <c r="B35" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" t="s">
-        <v>132</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" t="s">
-        <v>133</v>
-      </c>
-      <c r="G35" t="s">
-        <v>134</v>
-      </c>
-      <c r="H35" t="s">
-        <v>15</v>
-      </c>
-      <c r="I35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>136</v>
-      </c>
-      <c r="B36" t="s">
-        <v>137</v>
-      </c>
-      <c r="C36" t="s">
-        <v>138</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" t="s">
-        <v>137</v>
-      </c>
-      <c r="G36" t="s">
-        <v>139</v>
-      </c>
-      <c r="H36" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>141</v>
-      </c>
-      <c r="B37" t="s">
-        <v>174</v>
-      </c>
-      <c r="C37" t="s">
-        <v>175</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" t="s">
-        <v>174</v>
-      </c>
-      <c r="G37" t="s">
-        <v>48</v>
-      </c>
-      <c r="H37" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>142</v>
-      </c>
-      <c r="B38" t="s">
-        <v>143</v>
-      </c>
-      <c r="C38" t="s">
-        <v>144</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" t="s">
-        <v>145</v>
-      </c>
-      <c r="G38" t="s">
-        <v>70</v>
-      </c>
-      <c r="H38" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>